<commit_message>
Kevin en Bram scrum
</commit_message>
<xml_diff>
--- a/scrum/dailyscrum.xlsx
+++ b/scrum/dailyscrum.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bram\Documents\GitHub\project-appdev\scrum\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="26-02-2016" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="02-03-2016" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
+    <sheet name="26-02-2016" sheetId="2" r:id="rId2"/>
+    <sheet name="02-03-2016" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,30 +26,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
-  <si>
-    <t xml:space="preserve">Datum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rudy Mas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joran Claessens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kevin Strijbos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sacha Reyskens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bram Van Vleymen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frédérique Van Wonterghem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wat heb je gedaan?</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Rudy Mas</t>
+  </si>
+  <si>
+    <t>Joran Claessens</t>
+  </si>
+  <si>
+    <t>Kevin Strijbos</t>
+  </si>
+  <si>
+    <t>Sacha Reyskens</t>
+  </si>
+  <si>
+    <t>Bram Van Vleymen</t>
+  </si>
+  <si>
+    <t>Frédérique Van Wonterghem</t>
+  </si>
+  <si>
+    <t>Wat heb je gedaan?</t>
   </si>
   <si>
     <t xml:space="preserve">Wat ga je doen? </t>
@@ -54,75 +58,62 @@
     <t xml:space="preserve">Wat zijn je problemen? </t>
   </si>
   <si>
-    <t xml:space="preserve">GitHub Bekeken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope.md geschreven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Github volledig doorlopen, snap het nu perfect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Github bekeken, scum template gemaakt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GitHub bekeken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use Case “Eventlijst van standpunt student”
+    <t>GitHub Bekeken</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>scope.md geschreven</t>
+  </si>
+  <si>
+    <t>Github volledig doorlopen, snap het nu perfect</t>
+  </si>
+  <si>
+    <t>Github bekeken, scum template gemaakt.</t>
+  </si>
+  <si>
+    <t>GitHub bekeken</t>
+  </si>
+  <si>
+    <t>Use Case “Eventlijst van standpunt student”
 Beschrijving Pagina “Eventlijst”
 Beschrijving JavaScript / Jquery (Bootstrap)
 Facebook Info Doornemen</t>
   </si>
   <si>
-    <t xml:space="preserve">Use case “vervoersysteem”, beschrijving websitepagina “Vervoersysteem”, beschrijving HTML5 / CSS3, doornemen cursus Facebook API</t>
-  </si>
-  <si>
-    <t xml:space="preserve">use case "eventrating, student kan een event een waardering geven", gitignore onderzoeken, sql server in de cloud onderzoeken, beschrijving home/newsfeed pagina, beschrijving asp.net mvc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use case controle van organisatie + reviews, Beschrijving van profiel pagina organisatie, Bestuderen van ADO.Net SQL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use case Aanwezigheidsstatistieken (De raadpleging van de aanwezigheid). Statistiekenpagina beschrijven. Twitter API doornemen en beschrijven. Facebook api crusus doornemen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use case maken over het filteringsysteem en mutual friends, een paginabeschrijving over het filteringsysteem en het de Facebook API bespreken</t>
+    <t>Use case “vervoersysteem”, beschrijving websitepagina “Vervoersysteem”, beschrijving HTML5 / CSS3, doornemen cursus Facebook API</t>
+  </si>
+  <si>
+    <t>use case "eventrating, student kan een event een waardering geven", gitignore onderzoeken, sql server in de cloud onderzoeken, beschrijving home/newsfeed pagina, beschrijving asp.net mvc</t>
+  </si>
+  <si>
+    <t>Use case controle van organisatie + reviews, Beschrijving van profiel pagina organisatie, Bestuderen van ADO.Net SQL</t>
+  </si>
+  <si>
+    <t>Use case Aanwezigheidsstatistieken (De raadpleging van de aanwezigheid). Statistiekenpagina beschrijven. Twitter API doornemen en beschrijven. Facebook api crusus doornemen.</t>
+  </si>
+  <si>
+    <t>Use case maken over het filteringsysteem en mutual friends, een paginabeschrijving over het filteringsysteem en het de Facebook API bespreken</t>
+  </si>
+  <si>
+    <t>Visio diagrammen samenvoegen en generaliseren + inleiding database</t>
+  </si>
+  <si>
+    <t>contextdiagram maken, agendapunten voorbereiden en werkjes controleren</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="D/MMM/YY"/>
-  </numFmts>
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="18"/>
@@ -175,95 +166,74 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -322,31 +292,305 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="21.2755102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.6122448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="21.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.63775510204082"/>
+    <col min="1" max="6" width="21.21875"/>
+    <col min="7" max="7" width="32.5546875"/>
+    <col min="8" max="9" width="21.21875"/>
+    <col min="10" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -357,7 +601,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -378,7 +622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="121.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -389,7 +633,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="143.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:7" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -400,7 +644,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="104.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -415,37 +659,29 @@
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="21.2755102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.6122448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="21.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.63775510204082"/>
+    <col min="1" max="6" width="21.21875"/>
+    <col min="7" max="7" width="32.5546875"/>
+    <col min="8" max="9" width="21.21875"/>
+    <col min="10" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="n">
+    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
         <v>42426</v>
       </c>
       <c r="B1" s="1"/>
@@ -455,7 +691,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -476,7 +712,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="121.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -499,7 +735,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="143.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:7" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -522,7 +758,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="104.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -543,10 +779,9 @@
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Standaard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standaard"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -554,26 +789,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="21.2755102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.6122448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="21.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.63775510204082"/>
+    <col min="1" max="6" width="21.21875"/>
+    <col min="7" max="7" width="32.5546875"/>
+    <col min="8" max="9" width="21.21875"/>
+    <col min="10" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="n">
+    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
         <v>42431</v>
       </c>
       <c r="B1" s="1"/>
@@ -583,7 +815,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -604,29 +836,37 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="121.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="143.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:7" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="104.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -641,12 +881,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aanpassing verslag + dailyscrum
</commit_message>
<xml_diff>
--- a/scrum/dailyscrum.xlsx
+++ b/scrum/dailyscrum.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bram\Documents\GitHub\project-appdev\scrum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fred\Documents\GitHub\project-appdev\AppDev05_2016\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="989" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>Datum</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>docx bestanden omgezet naar md.</t>
+  </si>
+  <si>
+    <t>Afmaken Facebook API + bundelen paginabeschrijvingen</t>
   </si>
 </sst>
 </file>
@@ -232,9 +235,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="15" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -253,9 +253,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -339,9 +342,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -379,7 +382,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -451,7 +454,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -607,77 +610,77 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="22"/>
-    <col min="7" max="7" width="33.44140625"/>
+    <col min="7" max="7" width="33.42578125"/>
     <col min="8" max="9" width="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:7" ht="121.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -693,110 +696,110 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="22"/>
-    <col min="7" max="7" width="33.44140625"/>
+    <col min="7" max="7" width="33.42578125"/>
     <col min="8" max="9" width="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="7">
         <v>42426</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:7" ht="121.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:7" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:7" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -816,106 +819,110 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="22"/>
-    <col min="7" max="7" width="33.44140625"/>
+    <col min="7" max="7" width="33.42578125"/>
     <col min="8" max="9" width="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="7">
         <v>42431</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:7" ht="121.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="G3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="G4" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="6"/>
+      <c r="G5" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -934,79 +941,79 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="22"/>
-    <col min="7" max="7" width="33.44140625"/>
+    <col min="7" max="7" width="33.42578125"/>
     <col min="8" max="9" width="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="7">
         <v>42433</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:7" ht="121.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>